<commit_message>
timerecording added new times
</commit_message>
<xml_diff>
--- a/Zeiterfassung.xlsx
+++ b/Zeiterfassung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\4Schuhljahr\Syp\Projekt\Multiflex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{050E9ECF-D677-4B59-9DA3-311B897FD007}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AF5D659-E052-4599-B4BB-C17B6691B82C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView showSheetTabs="0" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="25">
   <si>
     <t>Arbeitsstunden</t>
   </si>
@@ -98,6 +98,21 @@
   </si>
   <si>
     <t>Gesamte Stunden:</t>
+  </si>
+  <si>
+    <t>Dependences</t>
+  </si>
+  <si>
+    <t>Java Dependencies</t>
+  </si>
+  <si>
+    <t>Locale Datenbank testen</t>
+  </si>
+  <si>
+    <t>Frontend &amp; Database</t>
+  </si>
+  <si>
+    <t>Api und Frontend</t>
   </si>
 </sst>
 </file>
@@ -164,7 +179,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="33">
+  <borders count="36">
     <border>
       <left/>
       <right/>
@@ -562,11 +577,46 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="dotted">
+        <color auto="1"/>
+      </right>
+      <top style="dotted">
+        <color auto="1"/>
+      </top>
+      <bottom style="dotted">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -647,10 +697,78 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="3" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="28" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="30" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -669,24 +787,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -704,6 +804,18 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -721,6 +833,12 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -736,28 +854,31 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="3" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="28" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="30" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1130,10 +1251,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AC25"/>
+  <dimension ref="A1:AC29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="S30" sqref="S30"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="K4" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="U27" sqref="U27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1146,66 +1267,70 @@
     <col min="8" max="8" width="19.140625" style="2" customWidth="1"/>
     <col min="9" max="9" width="1.28515625" style="2" customWidth="1"/>
     <col min="10" max="10" width="14.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="18" width="10.85546875" style="2"/>
+    <col min="11" max="14" width="10.85546875" style="2"/>
+    <col min="15" max="15" width="14.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="10.85546875" style="2"/>
     <col min="19" max="19" width="14.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="27" width="10.85546875" style="2"/>
+    <col min="20" max="23" width="10.85546875" style="2"/>
+    <col min="24" max="24" width="14.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="25" max="27" width="10.85546875" style="2"/>
     <col min="28" max="28" width="18" style="2" bestFit="1" customWidth="1"/>
     <col min="29" max="16384" width="10.85546875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="1" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="46"/>
-      <c r="P1" s="46"/>
-      <c r="Q1" s="46"/>
-      <c r="R1" s="46"/>
-      <c r="S1" s="46"/>
-      <c r="T1" s="46"/>
-      <c r="U1" s="46"/>
-      <c r="V1" s="46"/>
-      <c r="W1" s="46"/>
-      <c r="X1" s="46"/>
-      <c r="Y1" s="46"/>
-      <c r="Z1" s="46"/>
-      <c r="AA1" s="46"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="66"/>
+      <c r="K1" s="66"/>
+      <c r="L1" s="66"/>
+      <c r="M1" s="66"/>
+      <c r="N1" s="66"/>
+      <c r="O1" s="66"/>
+      <c r="P1" s="66"/>
+      <c r="Q1" s="66"/>
+      <c r="R1" s="66"/>
+      <c r="S1" s="66"/>
+      <c r="T1" s="66"/>
+      <c r="U1" s="66"/>
+      <c r="V1" s="66"/>
+      <c r="W1" s="66"/>
+      <c r="X1" s="66"/>
+      <c r="Y1" s="66"/>
+      <c r="Z1" s="66"/>
+      <c r="AA1" s="66"/>
     </row>
     <row r="2" spans="1:29" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
-      <c r="B2" s="47"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="31" t="s">
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="29"/>
-      <c r="I2" s="30"/>
-      <c r="P2" s="50" t="s">
+      <c r="H2" s="51"/>
+      <c r="I2" s="52"/>
+      <c r="P2" s="72" t="s">
         <v>15</v>
       </c>
-      <c r="Q2" s="51"/>
-      <c r="R2" s="51"/>
-      <c r="Y2" s="31" t="s">
+      <c r="Q2" s="73"/>
+      <c r="R2" s="73"/>
+      <c r="Y2" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="Z2" s="29"/>
-      <c r="AA2" s="30"/>
+      <c r="Z2" s="51"/>
+      <c r="AA2" s="52"/>
     </row>
     <row r="3" spans="1:29" s="5" customFormat="1" ht="19.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
@@ -1226,11 +1351,11 @@
       <c r="F3" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="G3" s="38" t="s">
+      <c r="G3" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="38"/>
-      <c r="I3" s="39"/>
+      <c r="H3" s="61"/>
+      <c r="I3" s="62"/>
       <c r="J3" s="9" t="s">
         <v>9</v>
       </c>
@@ -1249,11 +1374,11 @@
       <c r="O3" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="P3" s="38" t="s">
+      <c r="P3" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="Q3" s="38"/>
-      <c r="R3" s="39"/>
+      <c r="Q3" s="61"/>
+      <c r="R3" s="62"/>
       <c r="S3" s="13" t="s">
         <v>8</v>
       </c>
@@ -1272,15 +1397,15 @@
       <c r="X3" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="Y3" s="38" t="s">
+      <c r="Y3" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="Z3" s="38"/>
-      <c r="AA3" s="39"/>
-      <c r="AB3" s="62" t="s">
+      <c r="Z3" s="61"/>
+      <c r="AA3" s="62"/>
+      <c r="AB3" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="AC3" s="61">
+      <c r="AC3" s="26">
         <f>SUM(X10+O10+F9)</f>
         <v>1.1979166666666665</v>
       </c>
@@ -1303,11 +1428,11 @@
         <f>D4-C4-E4</f>
         <v>7.2916666666666685E-2</v>
       </c>
-      <c r="G4" s="40" t="s">
+      <c r="G4" s="56" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="40"/>
-      <c r="I4" s="41"/>
+      <c r="H4" s="56"/>
+      <c r="I4" s="57"/>
       <c r="J4" s="23" t="s">
         <v>9</v>
       </c>
@@ -1325,11 +1450,11 @@
         <f t="shared" ref="O4:O9" si="0">M4-L4-N4</f>
         <v>7.2916666666666685E-2</v>
       </c>
-      <c r="P4" s="40" t="s">
+      <c r="P4" s="56" t="s">
         <v>10</v>
       </c>
-      <c r="Q4" s="40"/>
-      <c r="R4" s="41"/>
+      <c r="Q4" s="56"/>
+      <c r="R4" s="57"/>
       <c r="S4" s="23" t="s">
         <v>8</v>
       </c>
@@ -1347,11 +1472,11 @@
         <f t="shared" ref="X4:X9" si="1">V4-U4-W4</f>
         <v>7.2916666666666685E-2</v>
       </c>
-      <c r="Y4" s="40" t="s">
+      <c r="Y4" s="56" t="s">
         <v>10</v>
       </c>
-      <c r="Z4" s="40"/>
-      <c r="AA4" s="41"/>
+      <c r="Z4" s="56"/>
+      <c r="AA4" s="57"/>
     </row>
     <row r="5" spans="1:29" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
@@ -1371,11 +1496,11 @@
         <f>D5-C5-E5</f>
         <v>0.20833333333333337</v>
       </c>
-      <c r="G5" s="32" t="s">
+      <c r="G5" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="32"/>
-      <c r="I5" s="33"/>
+      <c r="H5" s="54"/>
+      <c r="I5" s="55"/>
       <c r="J5" s="23" t="s">
         <v>9</v>
       </c>
@@ -1393,11 +1518,11 @@
         <f t="shared" si="0"/>
         <v>7.2916666666666685E-2</v>
       </c>
-      <c r="P5" s="36" t="s">
+      <c r="P5" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="Q5" s="36"/>
-      <c r="R5" s="37"/>
+      <c r="Q5" s="63"/>
+      <c r="R5" s="64"/>
       <c r="S5" s="23" t="s">
         <v>8</v>
       </c>
@@ -1415,11 +1540,11 @@
         <f t="shared" si="1"/>
         <v>0.20833333333333326</v>
       </c>
-      <c r="Y5" s="32" t="s">
+      <c r="Y5" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="Z5" s="32"/>
-      <c r="AA5" s="33"/>
+      <c r="Z5" s="54"/>
+      <c r="AA5" s="55"/>
     </row>
     <row r="6" spans="1:29" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
@@ -1439,11 +1564,11 @@
         <f>D6-C6-E6</f>
         <v>7.2916666666666685E-2</v>
       </c>
-      <c r="G6" s="32" t="s">
+      <c r="G6" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="32"/>
-      <c r="I6" s="33"/>
+      <c r="H6" s="54"/>
+      <c r="I6" s="55"/>
       <c r="J6" s="23" t="s">
         <v>9</v>
       </c>
@@ -1461,9 +1586,9 @@
         <f t="shared" si="0"/>
         <v>3.472222222222221E-2</v>
       </c>
-      <c r="P6" s="36"/>
-      <c r="Q6" s="36"/>
-      <c r="R6" s="37"/>
+      <c r="P6" s="63"/>
+      <c r="Q6" s="63"/>
+      <c r="R6" s="64"/>
       <c r="S6" s="23" t="s">
         <v>8</v>
       </c>
@@ -1481,11 +1606,11 @@
         <f t="shared" si="1"/>
         <v>7.2916666666666685E-2</v>
       </c>
-      <c r="Y6" s="36" t="s">
+      <c r="Y6" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="Z6" s="36"/>
-      <c r="AA6" s="37"/>
+      <c r="Z6" s="63"/>
+      <c r="AA6" s="64"/>
     </row>
     <row r="7" spans="1:29" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
@@ -1505,11 +1630,11 @@
         <f>D7-C7-E7</f>
         <v>3.472222222222221E-2</v>
       </c>
-      <c r="G7" s="32" t="s">
+      <c r="G7" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="32"/>
-      <c r="I7" s="33"/>
+      <c r="H7" s="54"/>
+      <c r="I7" s="55"/>
       <c r="J7" s="23" t="s">
         <v>9</v>
       </c>
@@ -1527,9 +1652,9 @@
         <f t="shared" si="0"/>
         <v>3.472222222222221E-2</v>
       </c>
-      <c r="P7" s="36"/>
-      <c r="Q7" s="36"/>
-      <c r="R7" s="37"/>
+      <c r="P7" s="63"/>
+      <c r="Q7" s="63"/>
+      <c r="R7" s="64"/>
       <c r="S7" s="23" t="s">
         <v>8</v>
       </c>
@@ -1547,9 +1672,9 @@
         <f t="shared" si="1"/>
         <v>3.472222222222221E-2</v>
       </c>
-      <c r="Y7" s="36"/>
-      <c r="Z7" s="36"/>
-      <c r="AA7" s="37"/>
+      <c r="Y7" s="63"/>
+      <c r="Z7" s="63"/>
+      <c r="AA7" s="64"/>
     </row>
     <row r="8" spans="1:29" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
@@ -1569,11 +1694,11 @@
         <f>D8-C8-E8</f>
         <v>3.472222222222221E-2</v>
       </c>
-      <c r="G8" s="34" t="s">
+      <c r="G8" s="70" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="34"/>
-      <c r="I8" s="35"/>
+      <c r="H8" s="70"/>
+      <c r="I8" s="71"/>
       <c r="J8" s="23" t="s">
         <v>9</v>
       </c>
@@ -1591,11 +1716,11 @@
         <f t="shared" si="0"/>
         <v>3.125E-2</v>
       </c>
-      <c r="P8" s="36" t="s">
+      <c r="P8" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="Q8" s="36"/>
-      <c r="R8" s="37"/>
+      <c r="Q8" s="63"/>
+      <c r="R8" s="64"/>
       <c r="S8" s="23" t="s">
         <v>8</v>
       </c>
@@ -1613,9 +1738,9 @@
         <f t="shared" si="1"/>
         <v>3.472222222222221E-2</v>
       </c>
-      <c r="Y8" s="36"/>
-      <c r="Z8" s="36"/>
-      <c r="AA8" s="37"/>
+      <c r="Y8" s="63"/>
+      <c r="Z8" s="63"/>
+      <c r="AA8" s="64"/>
     </row>
     <row r="9" spans="1:29" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F9" s="6">
@@ -1639,11 +1764,11 @@
         <f t="shared" si="0"/>
         <v>0.125</v>
       </c>
-      <c r="P9" s="26" t="s">
+      <c r="P9" s="77" t="s">
         <v>12</v>
       </c>
-      <c r="Q9" s="26"/>
-      <c r="R9" s="27"/>
+      <c r="Q9" s="77"/>
+      <c r="R9" s="78"/>
       <c r="S9" s="24" t="s">
         <v>8</v>
       </c>
@@ -1661,11 +1786,11 @@
         <f t="shared" si="1"/>
         <v>0.125</v>
       </c>
-      <c r="Y9" s="26" t="s">
+      <c r="Y9" s="77" t="s">
         <v>12</v>
       </c>
-      <c r="Z9" s="26"/>
-      <c r="AA9" s="27"/>
+      <c r="Z9" s="77"/>
+      <c r="AA9" s="78"/>
     </row>
     <row r="10" spans="1:29" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="G10" s="8"/>
@@ -1704,58 +1829,70 @@
       <c r="R12" s="4"/>
     </row>
     <row r="13" spans="1:29" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="45" t="s">
+      <c r="A13" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="B13" s="46"/>
-      <c r="C13" s="46"/>
-      <c r="D13" s="46"/>
-      <c r="E13" s="46"/>
-      <c r="F13" s="46"/>
-      <c r="G13" s="46"/>
-      <c r="H13" s="46"/>
-      <c r="I13" s="46"/>
-      <c r="J13" s="46"/>
-      <c r="K13" s="46"/>
-      <c r="L13" s="46"/>
-      <c r="M13" s="46"/>
-      <c r="N13" s="46"/>
-      <c r="O13" s="46"/>
-      <c r="P13" s="46"/>
-      <c r="Q13" s="46"/>
-      <c r="R13" s="46"/>
-      <c r="S13" s="46"/>
-      <c r="T13" s="46"/>
-      <c r="U13" s="46"/>
-      <c r="V13" s="46"/>
-      <c r="W13" s="46"/>
-      <c r="X13" s="46"/>
-      <c r="Y13" s="46"/>
-      <c r="Z13" s="46"/>
-      <c r="AA13" s="46"/>
+      <c r="B13" s="66"/>
+      <c r="C13" s="66"/>
+      <c r="D13" s="66"/>
+      <c r="E13" s="66"/>
+      <c r="F13" s="66"/>
+      <c r="G13" s="66"/>
+      <c r="H13" s="66"/>
+      <c r="I13" s="66"/>
+      <c r="J13" s="66"/>
+      <c r="K13" s="66"/>
+      <c r="L13" s="66"/>
+      <c r="M13" s="66"/>
+      <c r="N13" s="66"/>
+      <c r="O13" s="66"/>
+      <c r="P13" s="66"/>
+      <c r="Q13" s="66"/>
+      <c r="R13" s="66"/>
+      <c r="S13" s="66"/>
+      <c r="T13" s="66"/>
+      <c r="U13" s="66"/>
+      <c r="V13" s="66"/>
+      <c r="W13" s="66"/>
+      <c r="X13" s="66"/>
+      <c r="Y13" s="66"/>
+      <c r="Z13" s="66"/>
+      <c r="AA13" s="66"/>
     </row>
     <row r="14" spans="1:29" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
-      <c r="B14" s="47"/>
-      <c r="C14" s="47"/>
-      <c r="D14" s="48"/>
-      <c r="E14" s="48"/>
-      <c r="F14" s="49"/>
-      <c r="G14" s="28" t="s">
+      <c r="B14" s="67"/>
+      <c r="C14" s="67"/>
+      <c r="D14" s="68"/>
+      <c r="E14" s="68"/>
+      <c r="F14" s="69"/>
+      <c r="G14" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="H14" s="29"/>
-      <c r="I14" s="30"/>
-      <c r="P14" s="28" t="s">
+      <c r="H14" s="51"/>
+      <c r="I14" s="52"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="67"/>
+      <c r="L14" s="67"/>
+      <c r="M14" s="68"/>
+      <c r="N14" s="68"/>
+      <c r="O14" s="69"/>
+      <c r="P14" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="Q14" s="29"/>
-      <c r="R14" s="30"/>
-      <c r="Y14" s="28" t="s">
+      <c r="Q14" s="51"/>
+      <c r="R14" s="52"/>
+      <c r="S14" s="7"/>
+      <c r="T14" s="67"/>
+      <c r="U14" s="67"/>
+      <c r="V14" s="68"/>
+      <c r="W14" s="68"/>
+      <c r="X14" s="69"/>
+      <c r="Y14" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="Z14" s="29"/>
-      <c r="AA14" s="30"/>
+      <c r="Z14" s="51"/>
+      <c r="AA14" s="52"/>
     </row>
     <row r="15" spans="1:29" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
@@ -1776,12 +1913,12 @@
       <c r="F15" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="G15" s="38" t="s">
+      <c r="G15" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="H15" s="38"/>
-      <c r="I15" s="39"/>
-      <c r="J15" s="9" t="s">
+      <c r="H15" s="61"/>
+      <c r="I15" s="62"/>
+      <c r="J15" s="85" t="s">
         <v>9</v>
       </c>
       <c r="K15" s="10" t="s">
@@ -1799,11 +1936,11 @@
       <c r="O15" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="P15" s="38" t="s">
+      <c r="P15" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="Q15" s="38"/>
-      <c r="R15" s="39"/>
+      <c r="Q15" s="61"/>
+      <c r="R15" s="62"/>
       <c r="S15" s="13" t="s">
         <v>8</v>
       </c>
@@ -1822,17 +1959,17 @@
       <c r="X15" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="Y15" s="38" t="s">
+      <c r="Y15" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="Z15" s="38"/>
-      <c r="AA15" s="39"/>
-      <c r="AB15" s="62" t="s">
+      <c r="Z15" s="61"/>
+      <c r="AA15" s="62"/>
+      <c r="AB15" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="AC15" s="61">
-        <f>SUM(X22+O22+F21)</f>
-        <v>0.97916666666666674</v>
+      <c r="AC15" s="26">
+        <f>SUM(X26+O26+F24)</f>
+        <v>4.0416666666666679</v>
       </c>
     </row>
     <row r="16" spans="1:29" ht="13.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
@@ -1853,33 +1990,33 @@
         <f>D16-C16-E16</f>
         <v>0.25000000000000006</v>
       </c>
-      <c r="G16" s="40" t="s">
+      <c r="G16" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="H16" s="40"/>
-      <c r="I16" s="41"/>
+      <c r="H16" s="56"/>
+      <c r="I16" s="57"/>
       <c r="J16" s="23" t="s">
         <v>9</v>
       </c>
       <c r="K16" s="15">
         <v>43090</v>
       </c>
-      <c r="L16" s="16">
-        <v>0.79166666666666663</v>
-      </c>
-      <c r="M16" s="16">
-        <v>0.97916666666666663</v>
-      </c>
-      <c r="N16" s="16"/>
+      <c r="L16" s="28">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="M16" s="28">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="N16" s="15"/>
       <c r="O16" s="17">
-        <f t="shared" ref="O16:O21" si="2">M16-L16-N16</f>
-        <v>0.1875</v>
-      </c>
-      <c r="P16" s="42" t="s">
+        <f t="shared" ref="O16:O18" si="2">M16-L16-N16</f>
+        <v>0.10416666666666663</v>
+      </c>
+      <c r="P16" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="Q16" s="43"/>
-      <c r="R16" s="44"/>
+      <c r="Q16" s="59"/>
+      <c r="R16" s="60"/>
       <c r="S16" s="23" t="s">
         <v>8</v>
       </c>
@@ -1887,7 +2024,7 @@
         <v>43090</v>
       </c>
       <c r="U16" s="16">
-        <v>0.35416666666666669</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="V16" s="16">
         <v>0.52083333333333337</v>
@@ -1895,29 +2032,37 @@
       <c r="W16" s="16"/>
       <c r="X16" s="17">
         <f t="shared" ref="X16:X21" si="3">V16-U16-W16</f>
-        <v>0.16666666666666669</v>
-      </c>
-      <c r="Y16" s="42" t="s">
+        <v>0.18750000000000006</v>
+      </c>
+      <c r="Y16" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="Z16" s="43"/>
-      <c r="AA16" s="44"/>
+      <c r="Z16" s="59"/>
+      <c r="AA16" s="60"/>
     </row>
     <row r="17" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B17" s="15"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="19"/>
+      <c r="B17" s="15">
+        <v>43098</v>
+      </c>
+      <c r="C17" s="16">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D17" s="16">
+        <v>0.75</v>
+      </c>
+      <c r="E17" s="16"/>
       <c r="F17" s="17">
-        <f t="shared" ref="F17:F20" si="4">D17-C17-E17</f>
-        <v>0</v>
-      </c>
-      <c r="G17" s="32"/>
-      <c r="H17" s="32"/>
-      <c r="I17" s="33"/>
+        <f t="shared" ref="F17:F21" si="4">D17-C17-E17</f>
+        <v>0.20833333333333337</v>
+      </c>
+      <c r="G17" s="54" t="s">
+        <v>17</v>
+      </c>
+      <c r="H17" s="54"/>
+      <c r="I17" s="55"/>
       <c r="J17" s="23" t="s">
         <v>9</v>
       </c>
@@ -1935,11 +2080,11 @@
         <f t="shared" si="2"/>
         <v>0.10416666666666663</v>
       </c>
-      <c r="P17" s="58" t="s">
+      <c r="P17" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="Q17" s="59"/>
-      <c r="R17" s="60"/>
+      <c r="Q17" s="46"/>
+      <c r="R17" s="47"/>
       <c r="S17" s="23" t="s">
         <v>8</v>
       </c>
@@ -1957,232 +2102,592 @@
         <f t="shared" si="3"/>
         <v>0.27083333333333337</v>
       </c>
-      <c r="Y17" s="52"/>
-      <c r="Z17" s="53"/>
-      <c r="AA17" s="54"/>
+      <c r="Y17" s="74"/>
+      <c r="Z17" s="75"/>
+      <c r="AA17" s="76"/>
     </row>
     <row r="18" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B18" s="15"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
+      <c r="B18" s="15">
+        <v>43104</v>
+      </c>
+      <c r="C18" s="16">
+        <v>0.375</v>
+      </c>
+      <c r="D18" s="16">
+        <v>0.5</v>
+      </c>
       <c r="E18" s="16"/>
       <c r="F18" s="17">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G18" s="32"/>
-      <c r="H18" s="32"/>
-      <c r="I18" s="33"/>
+        <v>0.125</v>
+      </c>
+      <c r="G18" s="56" t="s">
+        <v>17</v>
+      </c>
+      <c r="H18" s="56"/>
+      <c r="I18" s="57"/>
       <c r="J18" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="K18" s="15"/>
-      <c r="L18" s="16"/>
-      <c r="M18" s="16"/>
+      <c r="K18" s="15">
+        <v>43090</v>
+      </c>
+      <c r="L18" s="16">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="M18" s="16">
+        <v>0.97916666666666663</v>
+      </c>
       <c r="N18" s="16"/>
       <c r="O18" s="17">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P18" s="42"/>
-      <c r="Q18" s="43"/>
-      <c r="R18" s="44"/>
+        <v>0.1875</v>
+      </c>
+      <c r="P18" s="58" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q18" s="59"/>
+      <c r="R18" s="60"/>
       <c r="S18" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="T18" s="15"/>
-      <c r="V18" s="19"/>
+      <c r="T18" s="15">
+        <v>43096</v>
+      </c>
+      <c r="U18" s="16">
+        <v>0.4375</v>
+      </c>
+      <c r="V18" s="18">
+        <v>0.5625</v>
+      </c>
       <c r="W18" s="16"/>
       <c r="X18" s="17">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="Y18" s="55"/>
-      <c r="Z18" s="56"/>
-      <c r="AA18" s="57"/>
+        <v>0.125</v>
+      </c>
+      <c r="Y18" s="58" t="s">
+        <v>18</v>
+      </c>
+      <c r="Z18" s="59"/>
+      <c r="AA18" s="60"/>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="15"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
+      <c r="B19" s="15">
+        <v>43107</v>
+      </c>
+      <c r="C19" s="16">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D19" s="16">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="E19" s="19"/>
       <c r="F19" s="17">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G19" s="32"/>
-      <c r="H19" s="32"/>
-      <c r="I19" s="33"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="G19" s="56" t="s">
+        <v>17</v>
+      </c>
+      <c r="H19" s="56"/>
+      <c r="I19" s="57"/>
       <c r="J19" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="K19" s="15"/>
-      <c r="L19" s="16"/>
-      <c r="M19" s="16"/>
+      <c r="K19" s="15">
+        <v>43098</v>
+      </c>
+      <c r="L19" s="16">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="M19" s="16">
+        <v>0.69791666666666663</v>
+      </c>
       <c r="N19" s="16"/>
       <c r="O19" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P19" s="55"/>
-      <c r="Q19" s="56"/>
-      <c r="R19" s="57"/>
+        <f>M19-L19-N19</f>
+        <v>0.15625</v>
+      </c>
+      <c r="P19" s="58" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q19" s="59"/>
+      <c r="R19" s="60"/>
       <c r="S19" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="T19" s="15"/>
-      <c r="U19" s="16"/>
-      <c r="V19" s="16"/>
+      <c r="T19" s="15">
+        <v>43097</v>
+      </c>
+      <c r="U19" s="16">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="V19" s="16">
+        <v>0.58333333333333337</v>
+      </c>
       <c r="W19" s="16"/>
       <c r="X19" s="17">
         <f>V19-U19-W19</f>
-        <v>0</v>
-      </c>
-      <c r="Y19" s="55"/>
-      <c r="Z19" s="56"/>
-      <c r="AA19" s="57"/>
+        <v>0.12500000000000006</v>
+      </c>
+      <c r="Y19" s="58" t="s">
+        <v>18</v>
+      </c>
+      <c r="Z19" s="59"/>
+      <c r="AA19" s="60"/>
     </row>
-    <row r="20" spans="1:27" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="20" t="s">
+    <row r="20" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="21"/>
-      <c r="C20" s="22"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="22"/>
+      <c r="B20" s="35">
+        <v>43107</v>
+      </c>
+      <c r="C20" s="18">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D20" s="18">
+        <v>0.75</v>
+      </c>
+      <c r="E20" s="19"/>
       <c r="F20" s="17">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G20" s="34"/>
-      <c r="H20" s="34"/>
-      <c r="I20" s="35"/>
+        <v>0.16666666666666663</v>
+      </c>
+      <c r="G20" s="54" t="s">
+        <v>21</v>
+      </c>
+      <c r="H20" s="54"/>
+      <c r="I20" s="55"/>
       <c r="J20" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="K20" s="15"/>
-      <c r="L20" s="16"/>
-      <c r="M20" s="16"/>
+      <c r="K20" s="15">
+        <v>43107</v>
+      </c>
+      <c r="L20" s="16">
+        <v>0.40625</v>
+      </c>
+      <c r="M20" s="16">
+        <v>0.5</v>
+      </c>
       <c r="N20" s="16"/>
       <c r="O20" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P20" s="36"/>
-      <c r="Q20" s="36"/>
-      <c r="R20" s="37"/>
+        <f>M20-L20-N20</f>
+        <v>9.375E-2</v>
+      </c>
+      <c r="P20" s="58" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q20" s="59"/>
+      <c r="R20" s="60"/>
       <c r="S20" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="T20" s="15"/>
-      <c r="U20" s="16"/>
-      <c r="V20" s="16"/>
+      <c r="T20" s="15">
+        <v>43103</v>
+      </c>
+      <c r="U20" s="16">
+        <v>0.75</v>
+      </c>
+      <c r="V20" s="16">
+        <v>0.83333333333333337</v>
+      </c>
       <c r="W20" s="16"/>
       <c r="X20" s="17">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="Y20" s="55"/>
+        <v>8.333333333333337E-2</v>
+      </c>
+      <c r="Y20" s="56" t="s">
+        <v>17</v>
+      </c>
       <c r="Z20" s="56"/>
       <c r="AA20" s="57"/>
     </row>
-    <row r="21" spans="1:27" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F21" s="6">
-        <f>SUM(F16:F20)</f>
-        <v>0.25000000000000006</v>
-      </c>
-      <c r="J21" s="25" t="s">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A21" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="15">
+        <v>43108</v>
+      </c>
+      <c r="C21" s="18">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D21" s="18">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E21" s="19"/>
+      <c r="F21" s="17">
+        <f t="shared" si="4"/>
+        <v>0.16666666666666674</v>
+      </c>
+      <c r="G21" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="H21" s="40"/>
+      <c r="I21" s="41"/>
+      <c r="J21" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="K21" s="21"/>
-      <c r="L21" s="22"/>
-      <c r="M21" s="22"/>
-      <c r="N21" s="22"/>
+      <c r="K21" s="15">
+        <v>43107</v>
+      </c>
+      <c r="L21" s="16">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="M21" s="16">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="N21" s="16"/>
       <c r="O21" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P21" s="26"/>
-      <c r="Q21" s="26"/>
-      <c r="R21" s="27"/>
-      <c r="S21" s="25" t="s">
+        <f>M21-L21-N21</f>
+        <v>0.20833333333333326</v>
+      </c>
+      <c r="P21" s="45" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q21" s="46"/>
+      <c r="R21" s="47"/>
+      <c r="S21" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="T21" s="21"/>
-      <c r="U21" s="22"/>
-      <c r="V21" s="22"/>
-      <c r="W21" s="22"/>
+      <c r="T21" s="15">
+        <v>43106</v>
+      </c>
+      <c r="U21" s="16">
+        <v>0.625</v>
+      </c>
+      <c r="V21" s="16">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="W21" s="16"/>
       <c r="X21" s="17">
         <f t="shared" si="3"/>
+        <v>8.333333333333337E-2</v>
+      </c>
+      <c r="Y21" s="79" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z21" s="79"/>
+      <c r="AA21" s="80"/>
+    </row>
+    <row r="22" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="35">
+        <v>43111</v>
+      </c>
+      <c r="C22" s="18">
+        <v>0.49305555555555558</v>
+      </c>
+      <c r="D22" s="18">
+        <v>0.52777777777777779</v>
+      </c>
+      <c r="E22" s="19"/>
+      <c r="F22" s="18">
+        <f>SUM(D22-C22)</f>
+        <v>3.472222222222221E-2</v>
+      </c>
+      <c r="G22" s="56" t="s">
+        <v>18</v>
+      </c>
+      <c r="H22" s="56"/>
+      <c r="I22" s="57"/>
+      <c r="J22" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="K22" s="15">
+        <v>43108</v>
+      </c>
+      <c r="L22" s="16">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="M22" s="16">
+        <v>0.875</v>
+      </c>
+      <c r="N22" s="16"/>
+      <c r="O22" s="17">
+        <f>M22-L22-N22</f>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="P22" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q22" s="40"/>
+      <c r="R22" s="41"/>
+      <c r="S22" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="T22" s="35">
+        <v>43111</v>
+      </c>
+      <c r="U22" s="18">
+        <v>0.49305555555555558</v>
+      </c>
+      <c r="V22" s="18">
+        <v>0.52777777777777779</v>
+      </c>
+      <c r="W22" s="19"/>
+      <c r="X22" s="18">
+        <f>SUM(V22-U22)</f>
+        <v>3.472222222222221E-2</v>
+      </c>
+      <c r="Y22" s="56" t="s">
+        <v>18</v>
+      </c>
+      <c r="Z22" s="56"/>
+      <c r="AA22" s="57"/>
+    </row>
+    <row r="23" spans="1:27" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="84">
+        <v>43112</v>
+      </c>
+      <c r="C23" s="36">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D23" s="36">
+        <v>0.625</v>
+      </c>
+      <c r="E23" s="37"/>
+      <c r="F23" s="18">
+        <f t="shared" ref="F23" si="5">SUM(D23-C23)</f>
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="G23" s="48" t="s">
+        <v>24</v>
+      </c>
+      <c r="H23" s="48"/>
+      <c r="I23" s="49"/>
+      <c r="J23" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="K23" s="15">
+        <v>43108</v>
+      </c>
+      <c r="L23" s="81">
+        <v>0.875</v>
+      </c>
+      <c r="M23" s="16">
+        <v>1</v>
+      </c>
+      <c r="N23" s="82"/>
+      <c r="O23" s="17">
+        <f>M23-L23-N23</f>
+        <v>0.125</v>
+      </c>
+      <c r="P23" s="45" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q23" s="46"/>
+      <c r="R23" s="47"/>
+      <c r="S23" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="T23" s="35">
+        <v>43111</v>
+      </c>
+      <c r="U23" s="18">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="V23" s="18">
+        <v>1</v>
+      </c>
+      <c r="W23" s="19"/>
+      <c r="X23" s="18">
+        <f>SUM(V23-U23)</f>
+        <v>8.333333333333337E-2</v>
+      </c>
+      <c r="Y23" s="79" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z23" s="79"/>
+      <c r="AA23" s="80"/>
+    </row>
+    <row r="24" spans="1:27" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F24" s="6">
+        <f>SUM(F16:F23)</f>
+        <v>1.3055555555555558</v>
+      </c>
+      <c r="J24" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="K24" s="35">
+        <v>43111</v>
+      </c>
+      <c r="L24" s="18">
+        <v>0.49305555555555558</v>
+      </c>
+      <c r="M24" s="18">
+        <v>0.52777777777777779</v>
+      </c>
+      <c r="N24" s="19"/>
+      <c r="O24" s="18">
+        <f>SUM(M24-L24)</f>
+        <v>3.472222222222221E-2</v>
+      </c>
+      <c r="P24" s="56" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q24" s="56"/>
+      <c r="R24" s="57"/>
+      <c r="S24" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="T24" s="35">
+        <v>43112</v>
+      </c>
+      <c r="U24" s="18">
         <v>0</v>
       </c>
-      <c r="Y21" s="26"/>
-      <c r="Z21" s="26"/>
-      <c r="AA21" s="27"/>
+      <c r="V24" s="18">
+        <v>0.125</v>
+      </c>
+      <c r="W24" s="19"/>
+      <c r="X24" s="18">
+        <f>SUM(V24-U24)</f>
+        <v>0.125</v>
+      </c>
+      <c r="Y24" s="79" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z24" s="79"/>
+      <c r="AA24" s="80"/>
     </row>
-    <row r="22" spans="1:27" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
-      <c r="L22" s="4"/>
-      <c r="M22" s="4"/>
-      <c r="O22" s="6">
-        <f>SUM(O16:O21)</f>
-        <v>0.29166666666666663</v>
-      </c>
-      <c r="P22" s="4"/>
-      <c r="Q22" s="4"/>
-      <c r="R22" s="4"/>
-      <c r="X22" s="6">
-        <f>SUM(X16:X21)</f>
-        <v>0.43750000000000006</v>
-      </c>
+    <row r="25" spans="1:27" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="J25" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="K25" s="84">
+        <v>43112</v>
+      </c>
+      <c r="L25" s="36">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="M25" s="36">
+        <v>0.625</v>
+      </c>
+      <c r="N25" s="37"/>
+      <c r="O25" s="18">
+        <f t="shared" ref="O25" si="6">SUM(M25-L25)</f>
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="P25" s="48" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q25" s="48"/>
+      <c r="R25" s="49"/>
+      <c r="S25" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="T25" s="83">
+        <v>43112</v>
+      </c>
+      <c r="U25" s="36">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="V25" s="36">
+        <v>0.625</v>
+      </c>
+      <c r="W25" s="37"/>
+      <c r="X25" s="18">
+        <f>SUM(V25-U25)</f>
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="Y25" s="48" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z25" s="48"/>
+      <c r="AA25" s="49"/>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B23" s="2"/>
+    <row r="26" spans="1:27" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="32"/>
+      <c r="C26" s="33"/>
+      <c r="D26" s="33"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="34"/>
+      <c r="G26" s="42"/>
+      <c r="H26" s="42"/>
+      <c r="I26" s="42"/>
+      <c r="K26" s="3"/>
+      <c r="O26" s="6">
+        <f>SUM(O16:O25)</f>
+        <v>1.3263888888888888</v>
+      </c>
+      <c r="X26" s="6">
+        <f>SUM(X16:X25)</f>
+        <v>1.4097222222222225</v>
+      </c>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B25" s="2"/>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="B28" s="29"/>
+      <c r="C28" s="30"/>
+      <c r="D28" s="30"/>
+      <c r="G28" s="43"/>
+      <c r="H28" s="43"/>
+      <c r="V28" s="30"/>
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="B29" s="31"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="30"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="44"/>
+      <c r="V29" s="30"/>
     </row>
   </sheetData>
-  <mergeCells count="47">
+  <mergeCells count="65">
+    <mergeCell ref="Y22:AA22"/>
+    <mergeCell ref="Y23:AA23"/>
+    <mergeCell ref="Y24:AA24"/>
+    <mergeCell ref="Y25:AA25"/>
     <mergeCell ref="Y19:AA19"/>
     <mergeCell ref="Y20:AA20"/>
     <mergeCell ref="P17:R17"/>
     <mergeCell ref="P19:R19"/>
-    <mergeCell ref="P18:R18"/>
     <mergeCell ref="G3:I3"/>
-    <mergeCell ref="A1:AA1"/>
-    <mergeCell ref="P2:R2"/>
-    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="Y18:AA18"/>
+    <mergeCell ref="P16:R16"/>
+    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="M14:O14"/>
+    <mergeCell ref="T14:U14"/>
+    <mergeCell ref="V14:X14"/>
     <mergeCell ref="Y16:AA17"/>
     <mergeCell ref="P3:R3"/>
     <mergeCell ref="Y3:AA3"/>
     <mergeCell ref="P4:R4"/>
     <mergeCell ref="P5:R7"/>
+    <mergeCell ref="Y9:AA9"/>
+    <mergeCell ref="P8:R8"/>
+    <mergeCell ref="P9:R9"/>
+    <mergeCell ref="Y5:AA5"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="A1:AA1"/>
+    <mergeCell ref="P2:R2"/>
+    <mergeCell ref="G2:I2"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:F2"/>
     <mergeCell ref="G4:I4"/>
-    <mergeCell ref="Y9:AA9"/>
-    <mergeCell ref="P8:R8"/>
-    <mergeCell ref="P9:R9"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="Y5:AA5"/>
     <mergeCell ref="G5:I5"/>
-    <mergeCell ref="Y18:AA18"/>
+    <mergeCell ref="A13:AA13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="D14:F14"/>
     <mergeCell ref="G14:I14"/>
     <mergeCell ref="P14:R14"/>
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="G21:I21"/>
     <mergeCell ref="P21:R21"/>
     <mergeCell ref="Y21:AA21"/>
     <mergeCell ref="Y14:AA14"/>
@@ -2195,10 +2700,18 @@
     <mergeCell ref="P15:R15"/>
     <mergeCell ref="Y15:AA15"/>
     <mergeCell ref="G16:I16"/>
-    <mergeCell ref="P16:R16"/>
+    <mergeCell ref="P18:R18"/>
     <mergeCell ref="Y4:AA4"/>
     <mergeCell ref="Y6:AA8"/>
-    <mergeCell ref="A13:AA13"/>
+    <mergeCell ref="P22:R22"/>
+    <mergeCell ref="P23:R23"/>
+    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="P25:R25"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="P24:R24"/>
+    <mergeCell ref="G22:I22"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>

<commit_message>
timerecording added new times fixes
</commit_message>
<xml_diff>
--- a/Zeiterfassung.xlsx
+++ b/Zeiterfassung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\4Schuhljahr\Syp\Projekt\Multiflex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AF5D659-E052-4599-B4BB-C17B6691B82C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8973C4B-F924-4A9F-98FD-E9006F4A8146}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView showSheetTabs="0" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -738,6 +738,131 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="20" fontId="3" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="28" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="30" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="26" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -755,131 +880,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="28" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="30" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="26" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="3" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1253,7 +1253,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="K4" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="115" workbookViewId="0">
       <selection activeCell="U27" sqref="U27"/>
     </sheetView>
   </sheetViews>
@@ -1279,58 +1279,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="1" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
-      <c r="J1" s="66"/>
-      <c r="K1" s="66"/>
-      <c r="L1" s="66"/>
-      <c r="M1" s="66"/>
-      <c r="N1" s="66"/>
-      <c r="O1" s="66"/>
-      <c r="P1" s="66"/>
-      <c r="Q1" s="66"/>
-      <c r="R1" s="66"/>
-      <c r="S1" s="66"/>
-      <c r="T1" s="66"/>
-      <c r="U1" s="66"/>
-      <c r="V1" s="66"/>
-      <c r="W1" s="66"/>
-      <c r="X1" s="66"/>
-      <c r="Y1" s="66"/>
-      <c r="Z1" s="66"/>
-      <c r="AA1" s="66"/>
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="73"/>
+      <c r="I1" s="73"/>
+      <c r="J1" s="73"/>
+      <c r="K1" s="73"/>
+      <c r="L1" s="73"/>
+      <c r="M1" s="73"/>
+      <c r="N1" s="73"/>
+      <c r="O1" s="73"/>
+      <c r="P1" s="73"/>
+      <c r="Q1" s="73"/>
+      <c r="R1" s="73"/>
+      <c r="S1" s="73"/>
+      <c r="T1" s="73"/>
+      <c r="U1" s="73"/>
+      <c r="V1" s="73"/>
+      <c r="W1" s="73"/>
+      <c r="X1" s="73"/>
+      <c r="Y1" s="73"/>
+      <c r="Z1" s="73"/>
+      <c r="AA1" s="73"/>
     </row>
     <row r="2" spans="1:29" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
-      <c r="B2" s="67"/>
-      <c r="C2" s="67"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="69"/>
-      <c r="G2" s="53" t="s">
+      <c r="B2" s="58"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="51"/>
-      <c r="I2" s="52"/>
-      <c r="P2" s="72" t="s">
+      <c r="H2" s="77"/>
+      <c r="I2" s="78"/>
+      <c r="P2" s="74" t="s">
         <v>15</v>
       </c>
-      <c r="Q2" s="73"/>
-      <c r="R2" s="73"/>
-      <c r="Y2" s="53" t="s">
+      <c r="Q2" s="75"/>
+      <c r="R2" s="75"/>
+      <c r="Y2" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="Z2" s="51"/>
-      <c r="AA2" s="52"/>
+      <c r="Z2" s="77"/>
+      <c r="AA2" s="78"/>
     </row>
     <row r="3" spans="1:29" s="5" customFormat="1" ht="19.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
@@ -1351,11 +1351,11 @@
       <c r="F3" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="G3" s="61" t="s">
+      <c r="G3" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="61"/>
-      <c r="I3" s="62"/>
+      <c r="H3" s="56"/>
+      <c r="I3" s="57"/>
       <c r="J3" s="9" t="s">
         <v>9</v>
       </c>
@@ -1374,11 +1374,11 @@
       <c r="O3" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="P3" s="61" t="s">
+      <c r="P3" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="Q3" s="61"/>
-      <c r="R3" s="62"/>
+      <c r="Q3" s="56"/>
+      <c r="R3" s="57"/>
       <c r="S3" s="13" t="s">
         <v>8</v>
       </c>
@@ -1397,11 +1397,11 @@
       <c r="X3" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="Y3" s="61" t="s">
+      <c r="Y3" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="Z3" s="61"/>
-      <c r="AA3" s="62"/>
+      <c r="Z3" s="56"/>
+      <c r="AA3" s="57"/>
       <c r="AB3" s="27" t="s">
         <v>19</v>
       </c>
@@ -1428,11 +1428,11 @@
         <f>D4-C4-E4</f>
         <v>7.2916666666666685E-2</v>
       </c>
-      <c r="G4" s="56" t="s">
+      <c r="G4" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="56"/>
-      <c r="I4" s="57"/>
+      <c r="H4" s="44"/>
+      <c r="I4" s="45"/>
       <c r="J4" s="23" t="s">
         <v>9</v>
       </c>
@@ -1450,11 +1450,11 @@
         <f t="shared" ref="O4:O9" si="0">M4-L4-N4</f>
         <v>7.2916666666666685E-2</v>
       </c>
-      <c r="P4" s="56" t="s">
+      <c r="P4" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="Q4" s="56"/>
-      <c r="R4" s="57"/>
+      <c r="Q4" s="44"/>
+      <c r="R4" s="45"/>
       <c r="S4" s="23" t="s">
         <v>8</v>
       </c>
@@ -1472,11 +1472,11 @@
         <f t="shared" ref="X4:X9" si="1">V4-U4-W4</f>
         <v>7.2916666666666685E-2</v>
       </c>
-      <c r="Y4" s="56" t="s">
+      <c r="Y4" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="Z4" s="56"/>
-      <c r="AA4" s="57"/>
+      <c r="Z4" s="44"/>
+      <c r="AA4" s="45"/>
     </row>
     <row r="5" spans="1:29" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
@@ -1496,11 +1496,11 @@
         <f>D5-C5-E5</f>
         <v>0.20833333333333337</v>
       </c>
-      <c r="G5" s="54" t="s">
+      <c r="G5" s="68" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="54"/>
-      <c r="I5" s="55"/>
+      <c r="H5" s="68"/>
+      <c r="I5" s="69"/>
       <c r="J5" s="23" t="s">
         <v>9</v>
       </c>
@@ -1518,11 +1518,11 @@
         <f t="shared" si="0"/>
         <v>7.2916666666666685E-2</v>
       </c>
-      <c r="P5" s="63" t="s">
+      <c r="P5" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="Q5" s="63"/>
-      <c r="R5" s="64"/>
+      <c r="Q5" s="64"/>
+      <c r="R5" s="65"/>
       <c r="S5" s="23" t="s">
         <v>8</v>
       </c>
@@ -1540,11 +1540,11 @@
         <f t="shared" si="1"/>
         <v>0.20833333333333326</v>
       </c>
-      <c r="Y5" s="54" t="s">
+      <c r="Y5" s="68" t="s">
         <v>11</v>
       </c>
-      <c r="Z5" s="54"/>
-      <c r="AA5" s="55"/>
+      <c r="Z5" s="68"/>
+      <c r="AA5" s="69"/>
     </row>
     <row r="6" spans="1:29" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
@@ -1564,11 +1564,11 @@
         <f>D6-C6-E6</f>
         <v>7.2916666666666685E-2</v>
       </c>
-      <c r="G6" s="54" t="s">
+      <c r="G6" s="68" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="54"/>
-      <c r="I6" s="55"/>
+      <c r="H6" s="68"/>
+      <c r="I6" s="69"/>
       <c r="J6" s="23" t="s">
         <v>9</v>
       </c>
@@ -1586,9 +1586,9 @@
         <f t="shared" si="0"/>
         <v>3.472222222222221E-2</v>
       </c>
-      <c r="P6" s="63"/>
-      <c r="Q6" s="63"/>
-      <c r="R6" s="64"/>
+      <c r="P6" s="64"/>
+      <c r="Q6" s="64"/>
+      <c r="R6" s="65"/>
       <c r="S6" s="23" t="s">
         <v>8</v>
       </c>
@@ -1606,11 +1606,11 @@
         <f t="shared" si="1"/>
         <v>7.2916666666666685E-2</v>
       </c>
-      <c r="Y6" s="63" t="s">
+      <c r="Y6" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="Z6" s="63"/>
-      <c r="AA6" s="64"/>
+      <c r="Z6" s="64"/>
+      <c r="AA6" s="65"/>
     </row>
     <row r="7" spans="1:29" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
@@ -1630,11 +1630,11 @@
         <f>D7-C7-E7</f>
         <v>3.472222222222221E-2</v>
       </c>
-      <c r="G7" s="54" t="s">
+      <c r="G7" s="68" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="54"/>
-      <c r="I7" s="55"/>
+      <c r="H7" s="68"/>
+      <c r="I7" s="69"/>
       <c r="J7" s="23" t="s">
         <v>9</v>
       </c>
@@ -1652,9 +1652,9 @@
         <f t="shared" si="0"/>
         <v>3.472222222222221E-2</v>
       </c>
-      <c r="P7" s="63"/>
-      <c r="Q7" s="63"/>
-      <c r="R7" s="64"/>
+      <c r="P7" s="64"/>
+      <c r="Q7" s="64"/>
+      <c r="R7" s="65"/>
       <c r="S7" s="23" t="s">
         <v>8</v>
       </c>
@@ -1672,9 +1672,9 @@
         <f t="shared" si="1"/>
         <v>3.472222222222221E-2</v>
       </c>
-      <c r="Y7" s="63"/>
-      <c r="Z7" s="63"/>
-      <c r="AA7" s="64"/>
+      <c r="Y7" s="64"/>
+      <c r="Z7" s="64"/>
+      <c r="AA7" s="65"/>
     </row>
     <row r="8" spans="1:29" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
@@ -1716,11 +1716,11 @@
         <f t="shared" si="0"/>
         <v>3.125E-2</v>
       </c>
-      <c r="P8" s="63" t="s">
+      <c r="P8" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="Q8" s="63"/>
-      <c r="R8" s="64"/>
+      <c r="Q8" s="64"/>
+      <c r="R8" s="65"/>
       <c r="S8" s="23" t="s">
         <v>8</v>
       </c>
@@ -1738,9 +1738,9 @@
         <f t="shared" si="1"/>
         <v>3.472222222222221E-2</v>
       </c>
-      <c r="Y8" s="63"/>
-      <c r="Z8" s="63"/>
-      <c r="AA8" s="64"/>
+      <c r="Y8" s="64"/>
+      <c r="Z8" s="64"/>
+      <c r="AA8" s="65"/>
     </row>
     <row r="9" spans="1:29" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F9" s="6">
@@ -1764,11 +1764,11 @@
         <f t="shared" si="0"/>
         <v>0.125</v>
       </c>
-      <c r="P9" s="77" t="s">
+      <c r="P9" s="66" t="s">
         <v>12</v>
       </c>
-      <c r="Q9" s="77"/>
-      <c r="R9" s="78"/>
+      <c r="Q9" s="66"/>
+      <c r="R9" s="67"/>
       <c r="S9" s="24" t="s">
         <v>8</v>
       </c>
@@ -1786,11 +1786,11 @@
         <f t="shared" si="1"/>
         <v>0.125</v>
       </c>
-      <c r="Y9" s="77" t="s">
+      <c r="Y9" s="66" t="s">
         <v>12</v>
       </c>
-      <c r="Z9" s="77"/>
-      <c r="AA9" s="78"/>
+      <c r="Z9" s="66"/>
+      <c r="AA9" s="67"/>
     </row>
     <row r="10" spans="1:29" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="G10" s="8"/>
@@ -1829,70 +1829,70 @@
       <c r="R12" s="4"/>
     </row>
     <row r="13" spans="1:29" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="65" t="s">
+      <c r="A13" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="B13" s="66"/>
-      <c r="C13" s="66"/>
-      <c r="D13" s="66"/>
-      <c r="E13" s="66"/>
-      <c r="F13" s="66"/>
-      <c r="G13" s="66"/>
-      <c r="H13" s="66"/>
-      <c r="I13" s="66"/>
-      <c r="J13" s="66"/>
-      <c r="K13" s="66"/>
-      <c r="L13" s="66"/>
-      <c r="M13" s="66"/>
-      <c r="N13" s="66"/>
-      <c r="O13" s="66"/>
-      <c r="P13" s="66"/>
-      <c r="Q13" s="66"/>
-      <c r="R13" s="66"/>
-      <c r="S13" s="66"/>
-      <c r="T13" s="66"/>
-      <c r="U13" s="66"/>
-      <c r="V13" s="66"/>
-      <c r="W13" s="66"/>
-      <c r="X13" s="66"/>
-      <c r="Y13" s="66"/>
-      <c r="Z13" s="66"/>
-      <c r="AA13" s="66"/>
+      <c r="B13" s="73"/>
+      <c r="C13" s="73"/>
+      <c r="D13" s="73"/>
+      <c r="E13" s="73"/>
+      <c r="F13" s="73"/>
+      <c r="G13" s="73"/>
+      <c r="H13" s="73"/>
+      <c r="I13" s="73"/>
+      <c r="J13" s="73"/>
+      <c r="K13" s="73"/>
+      <c r="L13" s="73"/>
+      <c r="M13" s="73"/>
+      <c r="N13" s="73"/>
+      <c r="O13" s="73"/>
+      <c r="P13" s="73"/>
+      <c r="Q13" s="73"/>
+      <c r="R13" s="73"/>
+      <c r="S13" s="73"/>
+      <c r="T13" s="73"/>
+      <c r="U13" s="73"/>
+      <c r="V13" s="73"/>
+      <c r="W13" s="73"/>
+      <c r="X13" s="73"/>
+      <c r="Y13" s="73"/>
+      <c r="Z13" s="73"/>
+      <c r="AA13" s="73"/>
     </row>
     <row r="14" spans="1:29" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
-      <c r="B14" s="67"/>
-      <c r="C14" s="67"/>
-      <c r="D14" s="68"/>
-      <c r="E14" s="68"/>
-      <c r="F14" s="69"/>
-      <c r="G14" s="50" t="s">
+      <c r="B14" s="58"/>
+      <c r="C14" s="58"/>
+      <c r="D14" s="59"/>
+      <c r="E14" s="59"/>
+      <c r="F14" s="60"/>
+      <c r="G14" s="79" t="s">
         <v>16</v>
       </c>
-      <c r="H14" s="51"/>
-      <c r="I14" s="52"/>
+      <c r="H14" s="77"/>
+      <c r="I14" s="78"/>
       <c r="J14" s="7"/>
-      <c r="K14" s="67"/>
-      <c r="L14" s="67"/>
-      <c r="M14" s="68"/>
-      <c r="N14" s="68"/>
-      <c r="O14" s="69"/>
-      <c r="P14" s="50" t="s">
+      <c r="K14" s="58"/>
+      <c r="L14" s="58"/>
+      <c r="M14" s="59"/>
+      <c r="N14" s="59"/>
+      <c r="O14" s="60"/>
+      <c r="P14" s="79" t="s">
         <v>16</v>
       </c>
-      <c r="Q14" s="51"/>
-      <c r="R14" s="52"/>
+      <c r="Q14" s="77"/>
+      <c r="R14" s="78"/>
       <c r="S14" s="7"/>
-      <c r="T14" s="67"/>
-      <c r="U14" s="67"/>
-      <c r="V14" s="68"/>
-      <c r="W14" s="68"/>
-      <c r="X14" s="69"/>
-      <c r="Y14" s="50" t="s">
+      <c r="T14" s="58"/>
+      <c r="U14" s="58"/>
+      <c r="V14" s="59"/>
+      <c r="W14" s="59"/>
+      <c r="X14" s="60"/>
+      <c r="Y14" s="79" t="s">
         <v>16</v>
       </c>
-      <c r="Z14" s="51"/>
-      <c r="AA14" s="52"/>
+      <c r="Z14" s="77"/>
+      <c r="AA14" s="78"/>
     </row>
     <row r="15" spans="1:29" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
@@ -1913,12 +1913,12 @@
       <c r="F15" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="G15" s="61" t="s">
+      <c r="G15" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="H15" s="61"/>
-      <c r="I15" s="62"/>
-      <c r="J15" s="85" t="s">
+      <c r="H15" s="56"/>
+      <c r="I15" s="57"/>
+      <c r="J15" s="43" t="s">
         <v>9</v>
       </c>
       <c r="K15" s="10" t="s">
@@ -1936,11 +1936,11 @@
       <c r="O15" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="P15" s="61" t="s">
+      <c r="P15" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="Q15" s="61"/>
-      <c r="R15" s="62"/>
+      <c r="Q15" s="56"/>
+      <c r="R15" s="57"/>
       <c r="S15" s="13" t="s">
         <v>8</v>
       </c>
@@ -1959,11 +1959,11 @@
       <c r="X15" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="Y15" s="61" t="s">
+      <c r="Y15" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="Z15" s="61"/>
-      <c r="AA15" s="62"/>
+      <c r="Z15" s="56"/>
+      <c r="AA15" s="57"/>
       <c r="AB15" s="27" t="s">
         <v>19</v>
       </c>
@@ -1990,11 +1990,11 @@
         <f>D16-C16-E16</f>
         <v>0.25000000000000006</v>
       </c>
-      <c r="G16" s="56" t="s">
+      <c r="G16" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="H16" s="56"/>
-      <c r="I16" s="57"/>
+      <c r="H16" s="44"/>
+      <c r="I16" s="45"/>
       <c r="J16" s="23" t="s">
         <v>9</v>
       </c>
@@ -2012,11 +2012,11 @@
         <f t="shared" ref="O16:O18" si="2">M16-L16-N16</f>
         <v>0.10416666666666663</v>
       </c>
-      <c r="P16" s="58" t="s">
+      <c r="P16" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="Q16" s="59"/>
-      <c r="R16" s="60"/>
+      <c r="Q16" s="51"/>
+      <c r="R16" s="52"/>
       <c r="S16" s="23" t="s">
         <v>8</v>
       </c>
@@ -2034,11 +2034,11 @@
         <f t="shared" ref="X16:X21" si="3">V16-U16-W16</f>
         <v>0.18750000000000006</v>
       </c>
-      <c r="Y16" s="58" t="s">
+      <c r="Y16" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="Z16" s="59"/>
-      <c r="AA16" s="60"/>
+      <c r="Z16" s="51"/>
+      <c r="AA16" s="52"/>
     </row>
     <row r="17" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="14" t="s">
@@ -2058,11 +2058,11 @@
         <f t="shared" ref="F17:F21" si="4">D17-C17-E17</f>
         <v>0.20833333333333337</v>
       </c>
-      <c r="G17" s="54" t="s">
+      <c r="G17" s="68" t="s">
         <v>17</v>
       </c>
-      <c r="H17" s="54"/>
-      <c r="I17" s="55"/>
+      <c r="H17" s="68"/>
+      <c r="I17" s="69"/>
       <c r="J17" s="23" t="s">
         <v>9</v>
       </c>
@@ -2080,11 +2080,11 @@
         <f t="shared" si="2"/>
         <v>0.10416666666666663</v>
       </c>
-      <c r="P17" s="45" t="s">
+      <c r="P17" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="Q17" s="46"/>
-      <c r="R17" s="47"/>
+      <c r="Q17" s="54"/>
+      <c r="R17" s="55"/>
       <c r="S17" s="23" t="s">
         <v>8</v>
       </c>
@@ -2102,9 +2102,9 @@
         <f t="shared" si="3"/>
         <v>0.27083333333333337</v>
       </c>
-      <c r="Y17" s="74"/>
-      <c r="Z17" s="75"/>
-      <c r="AA17" s="76"/>
+      <c r="Y17" s="61"/>
+      <c r="Z17" s="62"/>
+      <c r="AA17" s="63"/>
     </row>
     <row r="18" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="14" t="s">
@@ -2124,11 +2124,11 @@
         <f t="shared" si="4"/>
         <v>0.125</v>
       </c>
-      <c r="G18" s="56" t="s">
+      <c r="G18" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="H18" s="56"/>
-      <c r="I18" s="57"/>
+      <c r="H18" s="44"/>
+      <c r="I18" s="45"/>
       <c r="J18" s="23" t="s">
         <v>9</v>
       </c>
@@ -2146,11 +2146,11 @@
         <f t="shared" si="2"/>
         <v>0.1875</v>
       </c>
-      <c r="P18" s="58" t="s">
+      <c r="P18" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="Q18" s="59"/>
-      <c r="R18" s="60"/>
+      <c r="Q18" s="51"/>
+      <c r="R18" s="52"/>
       <c r="S18" s="23" t="s">
         <v>8</v>
       </c>
@@ -2168,11 +2168,11 @@
         <f t="shared" si="3"/>
         <v>0.125</v>
       </c>
-      <c r="Y18" s="58" t="s">
+      <c r="Y18" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="Z18" s="59"/>
-      <c r="AA18" s="60"/>
+      <c r="Z18" s="51"/>
+      <c r="AA18" s="52"/>
     </row>
     <row r="19" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="14" t="s">
@@ -2192,11 +2192,11 @@
         <f t="shared" si="4"/>
         <v>6.25E-2</v>
       </c>
-      <c r="G19" s="56" t="s">
+      <c r="G19" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="H19" s="56"/>
-      <c r="I19" s="57"/>
+      <c r="H19" s="44"/>
+      <c r="I19" s="45"/>
       <c r="J19" s="23" t="s">
         <v>9</v>
       </c>
@@ -2214,11 +2214,11 @@
         <f>M19-L19-N19</f>
         <v>0.15625</v>
       </c>
-      <c r="P19" s="58" t="s">
+      <c r="P19" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="Q19" s="59"/>
-      <c r="R19" s="60"/>
+      <c r="Q19" s="51"/>
+      <c r="R19" s="52"/>
       <c r="S19" s="23" t="s">
         <v>8</v>
       </c>
@@ -2236,11 +2236,11 @@
         <f>V19-U19-W19</f>
         <v>0.12500000000000006</v>
       </c>
-      <c r="Y19" s="58" t="s">
+      <c r="Y19" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="Z19" s="59"/>
-      <c r="AA19" s="60"/>
+      <c r="Z19" s="51"/>
+      <c r="AA19" s="52"/>
     </row>
     <row r="20" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="14" t="s">
@@ -2260,11 +2260,11 @@
         <f t="shared" si="4"/>
         <v>0.16666666666666663</v>
       </c>
-      <c r="G20" s="54" t="s">
+      <c r="G20" s="68" t="s">
         <v>21</v>
       </c>
-      <c r="H20" s="54"/>
-      <c r="I20" s="55"/>
+      <c r="H20" s="68"/>
+      <c r="I20" s="69"/>
       <c r="J20" s="23" t="s">
         <v>9</v>
       </c>
@@ -2282,11 +2282,11 @@
         <f>M20-L20-N20</f>
         <v>9.375E-2</v>
       </c>
-      <c r="P20" s="58" t="s">
+      <c r="P20" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="Q20" s="59"/>
-      <c r="R20" s="60"/>
+      <c r="Q20" s="51"/>
+      <c r="R20" s="52"/>
       <c r="S20" s="23" t="s">
         <v>8</v>
       </c>
@@ -2304,11 +2304,11 @@
         <f t="shared" si="3"/>
         <v>8.333333333333337E-2</v>
       </c>
-      <c r="Y20" s="56" t="s">
+      <c r="Y20" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="Z20" s="56"/>
-      <c r="AA20" s="57"/>
+      <c r="Z20" s="44"/>
+      <c r="AA20" s="45"/>
     </row>
     <row r="21" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A21" s="14" t="s">
@@ -2328,11 +2328,11 @@
         <f t="shared" si="4"/>
         <v>0.16666666666666674</v>
       </c>
-      <c r="G21" s="39" t="s">
+      <c r="G21" s="80" t="s">
         <v>22</v>
       </c>
-      <c r="H21" s="40"/>
-      <c r="I21" s="41"/>
+      <c r="H21" s="81"/>
+      <c r="I21" s="82"/>
       <c r="J21" s="23" t="s">
         <v>9</v>
       </c>
@@ -2350,11 +2350,11 @@
         <f>M21-L21-N21</f>
         <v>0.20833333333333326</v>
       </c>
-      <c r="P21" s="45" t="s">
+      <c r="P21" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="Q21" s="46"/>
-      <c r="R21" s="47"/>
+      <c r="Q21" s="54"/>
+      <c r="R21" s="55"/>
       <c r="S21" s="38" t="s">
         <v>8</v>
       </c>
@@ -2372,11 +2372,11 @@
         <f t="shared" si="3"/>
         <v>8.333333333333337E-2</v>
       </c>
-      <c r="Y21" s="79" t="s">
+      <c r="Y21" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="Z21" s="79"/>
-      <c r="AA21" s="80"/>
+      <c r="Z21" s="46"/>
+      <c r="AA21" s="47"/>
     </row>
     <row r="22" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="14" t="s">
@@ -2396,11 +2396,11 @@
         <f>SUM(D22-C22)</f>
         <v>3.472222222222221E-2</v>
       </c>
-      <c r="G22" s="56" t="s">
+      <c r="G22" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="H22" s="56"/>
-      <c r="I22" s="57"/>
+      <c r="H22" s="44"/>
+      <c r="I22" s="45"/>
       <c r="J22" s="38" t="s">
         <v>9</v>
       </c>
@@ -2418,11 +2418,11 @@
         <f>M22-L22-N22</f>
         <v>2.083333333333337E-2</v>
       </c>
-      <c r="P22" s="39" t="s">
+      <c r="P22" s="80" t="s">
         <v>14</v>
       </c>
-      <c r="Q22" s="40"/>
-      <c r="R22" s="41"/>
+      <c r="Q22" s="81"/>
+      <c r="R22" s="82"/>
       <c r="S22" s="23" t="s">
         <v>8</v>
       </c>
@@ -2440,17 +2440,17 @@
         <f>SUM(V22-U22)</f>
         <v>3.472222222222221E-2</v>
       </c>
-      <c r="Y22" s="56" t="s">
+      <c r="Y22" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="Z22" s="56"/>
-      <c r="AA22" s="57"/>
+      <c r="Z22" s="44"/>
+      <c r="AA22" s="45"/>
     </row>
     <row r="23" spans="1:27" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="B23" s="84">
+      <c r="B23" s="42">
         <v>43112</v>
       </c>
       <c r="C23" s="36">
@@ -2475,22 +2475,22 @@
       <c r="K23" s="15">
         <v>43108</v>
       </c>
-      <c r="L23" s="81">
+      <c r="L23" s="39">
         <v>0.875</v>
       </c>
       <c r="M23" s="16">
         <v>1</v>
       </c>
-      <c r="N23" s="82"/>
+      <c r="N23" s="40"/>
       <c r="O23" s="17">
         <f>M23-L23-N23</f>
         <v>0.125</v>
       </c>
-      <c r="P23" s="45" t="s">
+      <c r="P23" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="Q23" s="46"/>
-      <c r="R23" s="47"/>
+      <c r="Q23" s="54"/>
+      <c r="R23" s="55"/>
       <c r="S23" s="38" t="s">
         <v>8</v>
       </c>
@@ -2508,11 +2508,11 @@
         <f>SUM(V23-U23)</f>
         <v>8.333333333333337E-2</v>
       </c>
-      <c r="Y23" s="79" t="s">
+      <c r="Y23" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="Z23" s="79"/>
-      <c r="AA23" s="80"/>
+      <c r="Z23" s="46"/>
+      <c r="AA23" s="47"/>
     </row>
     <row r="24" spans="1:27" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F24" s="6">
@@ -2536,11 +2536,11 @@
         <f>SUM(M24-L24)</f>
         <v>3.472222222222221E-2</v>
       </c>
-      <c r="P24" s="56" t="s">
+      <c r="P24" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="Q24" s="56"/>
-      <c r="R24" s="57"/>
+      <c r="Q24" s="44"/>
+      <c r="R24" s="45"/>
       <c r="S24" s="38" t="s">
         <v>8</v>
       </c>
@@ -2558,17 +2558,17 @@
         <f>SUM(V24-U24)</f>
         <v>0.125</v>
       </c>
-      <c r="Y24" s="79" t="s">
+      <c r="Y24" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="Z24" s="79"/>
-      <c r="AA24" s="80"/>
+      <c r="Z24" s="46"/>
+      <c r="AA24" s="47"/>
     </row>
     <row r="25" spans="1:27" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="J25" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="K25" s="84">
+      <c r="K25" s="42">
         <v>43112</v>
       </c>
       <c r="L25" s="36">
@@ -2590,7 +2590,7 @@
       <c r="S25" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="T25" s="83">
+      <c r="T25" s="41">
         <v>43112</v>
       </c>
       <c r="U25" s="36">
@@ -2616,9 +2616,9 @@
       <c r="D26" s="33"/>
       <c r="E26" s="4"/>
       <c r="F26" s="34"/>
-      <c r="G26" s="42"/>
-      <c r="H26" s="42"/>
-      <c r="I26" s="42"/>
+      <c r="G26" s="83"/>
+      <c r="H26" s="83"/>
+      <c r="I26" s="83"/>
       <c r="K26" s="3"/>
       <c r="O26" s="6">
         <f>SUM(O16:O25)</f>
@@ -2633,26 +2633,63 @@
       <c r="B28" s="29"/>
       <c r="C28" s="30"/>
       <c r="D28" s="30"/>
-      <c r="G28" s="43"/>
-      <c r="H28" s="43"/>
+      <c r="G28" s="84"/>
+      <c r="H28" s="84"/>
       <c r="V28" s="30"/>
     </row>
     <row r="29" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B29" s="31"/>
       <c r="C29" s="30"/>
       <c r="D29" s="30"/>
-      <c r="G29" s="44"/>
-      <c r="H29" s="44"/>
+      <c r="G29" s="85"/>
+      <c r="H29" s="85"/>
       <c r="V29" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="65">
-    <mergeCell ref="Y22:AA22"/>
-    <mergeCell ref="Y23:AA23"/>
-    <mergeCell ref="Y24:AA24"/>
-    <mergeCell ref="Y25:AA25"/>
-    <mergeCell ref="Y19:AA19"/>
-    <mergeCell ref="Y20:AA20"/>
+    <mergeCell ref="P22:R22"/>
+    <mergeCell ref="P23:R23"/>
+    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="P25:R25"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="P24:R24"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="P21:R21"/>
+    <mergeCell ref="Y21:AA21"/>
+    <mergeCell ref="Y14:AA14"/>
+    <mergeCell ref="Y2:AA2"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="G19:I19"/>
+    <mergeCell ref="G20:I20"/>
+    <mergeCell ref="P20:R20"/>
+    <mergeCell ref="G15:I15"/>
+    <mergeCell ref="P15:R15"/>
+    <mergeCell ref="Y15:AA15"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="P18:R18"/>
+    <mergeCell ref="Y4:AA4"/>
+    <mergeCell ref="Y6:AA8"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="A13:AA13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="G14:I14"/>
+    <mergeCell ref="P14:R14"/>
+    <mergeCell ref="A1:AA1"/>
+    <mergeCell ref="P2:R2"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="P8:R8"/>
+    <mergeCell ref="P9:R9"/>
+    <mergeCell ref="Y5:AA5"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="G8:I8"/>
     <mergeCell ref="P17:R17"/>
     <mergeCell ref="P19:R19"/>
     <mergeCell ref="G3:I3"/>
@@ -2669,49 +2706,12 @@
     <mergeCell ref="P4:R4"/>
     <mergeCell ref="P5:R7"/>
     <mergeCell ref="Y9:AA9"/>
-    <mergeCell ref="P8:R8"/>
-    <mergeCell ref="P9:R9"/>
-    <mergeCell ref="Y5:AA5"/>
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="A1:AA1"/>
-    <mergeCell ref="P2:R2"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="A13:AA13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="P14:R14"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="P21:R21"/>
-    <mergeCell ref="Y21:AA21"/>
-    <mergeCell ref="Y14:AA14"/>
-    <mergeCell ref="Y2:AA2"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="G19:I19"/>
-    <mergeCell ref="G20:I20"/>
-    <mergeCell ref="P20:R20"/>
-    <mergeCell ref="G15:I15"/>
-    <mergeCell ref="P15:R15"/>
-    <mergeCell ref="Y15:AA15"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="P18:R18"/>
-    <mergeCell ref="Y4:AA4"/>
-    <mergeCell ref="Y6:AA8"/>
-    <mergeCell ref="P22:R22"/>
-    <mergeCell ref="P23:R23"/>
-    <mergeCell ref="G26:I26"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="P25:R25"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="P24:R24"/>
-    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="Y22:AA22"/>
+    <mergeCell ref="Y23:AA23"/>
+    <mergeCell ref="Y24:AA24"/>
+    <mergeCell ref="Y25:AA25"/>
+    <mergeCell ref="Y19:AA19"/>
+    <mergeCell ref="Y20:AA20"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>

<commit_message>
Zeitaufzeichnung Fixed gesamtZeit Bug
</commit_message>
<xml_diff>
--- a/Zeiterfassung.xlsx
+++ b/Zeiterfassung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\4Schuljahr\syp\Projekt\multiflexlbkv\multiflexlbkv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E68BE5F9-6F0F-4082-B06D-D503FEA93A60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E7D5D1D-6842-4725-8967-3A41CE0E9575}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView showSheetTabs="0" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12252" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2173,8 +2173,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BD154"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F125" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="J147" sqref="J147"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="U125" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="AB139" sqref="AB139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -9585,7 +9585,7 @@
         <v>19</v>
       </c>
       <c r="AC135" s="26">
-        <v>1.8680555555555556</v>
+        <v>2.0347222222222223</v>
       </c>
     </row>
     <row r="136" spans="1:29" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
@@ -9871,12 +9871,12 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="D140" s="18">
-        <v>0.625</v>
+        <v>0.79166666666666663</v>
       </c>
       <c r="E140" s="19"/>
       <c r="F140" s="18">
         <f>SUM(D140-C140)</f>
-        <v>8.333333333333337E-2</v>
+        <v>0.25</v>
       </c>
       <c r="G140" s="108" t="s">
         <v>53</v>
@@ -9993,8 +9993,8 @@
       <c r="D142" s="58"/>
       <c r="E142" s="4"/>
       <c r="F142" s="106">
-        <f ca="1">SUM(F135:F145)</f>
-        <v>0.61805555555555569</v>
+        <f>SUM(F135:F141)</f>
+        <v>0.78472222222222232</v>
       </c>
       <c r="G142" s="191"/>
       <c r="H142" s="191"/>

</xml_diff>